<commit_message>
se ajustan imports para probar ejecucion
</commit_message>
<xml_diff>
--- a/src/testData/AltaEmpleados.xlsx
+++ b/src/testData/AltaEmpleados.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -817,7 +817,7 @@
   <dimension ref="A1:BG6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>